<commit_message>
Incidencias y hoja de ruta
</commit_message>
<xml_diff>
--- a/Documentacion/MDSQL/Monitorización/Incidencias/Listado_Incidencias.xlsx
+++ b/Documentacion/MDSQL/Monitorización/Incidencias/Listado_Incidencias.xlsx
@@ -11,7 +11,8 @@
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hoja1!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hoja1!$A$1:$F$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hoja1!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -272,7 +273,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -305,21 +306,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -334,8 +320,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor rgb="FF008080"/>
+        <fgColor rgb="FFDDE8CB"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -373,7 +359,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -382,7 +368,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -390,28 +380,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -459,7 +433,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFDDE8CB"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -474,7 +448,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF00B050"/>
+      <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -497,14 +471,14 @@
   </sheetPr>
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="A34:F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="91.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.44"/>
@@ -545,107 +519,108 @@
       <c r="D2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="2" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E6" s="0" t="s">
+      <c r="D6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="D7" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -662,7 +637,8 @@
       <c r="D8" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -679,7 +655,8 @@
       <c r="D9" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -696,7 +673,8 @@
       <c r="D10" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -713,24 +691,26 @@
       <c r="D11" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" s="0" t="s">
+      <c r="B12" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -747,7 +727,8 @@
       <c r="D13" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -764,336 +745,352 @@
       <c r="D14" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="0" t="s">
+      <c r="D15" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="B18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="6" t="n">
+      <c r="D18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C19" s="0" t="s">
+      <c r="B19" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F19" s="0" t="s">
+      <c r="D19" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C20" s="0" t="s">
+      <c r="B20" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F20" s="0" t="s">
+      <c r="D20" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="6" t="n">
+      <c r="B22" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="6" t="n">
+      <c r="D22" s="2" t="n">
         <v>5</v>
       </c>
       <c r="E22" s="2"/>
-      <c r="F22" s="0" t="s">
+      <c r="F22" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C25" s="6" t="s">
+      <c r="B25" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C26" s="0" t="s">
+      <c r="B26" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F26" s="0" t="s">
+      <c r="D26" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="0" t="s">
+      <c r="B27" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F27" s="0" t="s">
+      <c r="D27" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="B28" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F28" s="0" t="s">
+      <c r="D28" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="B29" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="F29" s="0" t="s">
+      <c r="D29" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C30" s="7" t="s">
+      <c r="B30" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="F30" s="0" t="s">
+      <c r="D30" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="7" t="n">
+      <c r="D31" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="F31" s="0" t="s">
+      <c r="E31" s="4"/>
+      <c r="F31" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="0" t="n">
+      <c r="B32" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="7" t="n">
+      <c r="D32" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F32" s="0" t="s">
+      <c r="E32" s="4"/>
+      <c r="F32" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" s="0" t="s">
+      <c r="B33" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="0" t="n">
+      <c r="D33" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F33" s="0" t="s">
+      <c r="E33" s="2"/>
+      <c r="F33" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1110,58 +1107,62 @@
       <c r="D34" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F34" s="0" t="s">
+      <c r="E34" s="2"/>
+      <c r="F34" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F35" s="0" t="s">
+      <c r="E35" s="2"/>
+      <c r="F35" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C36" s="0" t="s">
+      <c r="B36" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="D36" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F36" s="0" t="s">
+      <c r="E36" s="2"/>
+      <c r="F36" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C37" s="0" t="s">
+      <c r="B37" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="0" t="n">
+      <c r="D37" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F37" s="0" t="s">
+      <c r="E37" s="2"/>
+      <c r="F37" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1178,160 +1179,170 @@
       <c r="D38" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F38" s="0" t="s">
+      <c r="E38" s="2"/>
+      <c r="F38" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D39" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F39" s="0" t="s">
+      <c r="D39" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C40" s="0" t="s">
+      <c r="B40" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F40" s="0" t="s">
+      <c r="D40" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="0" t="n">
+      <c r="B41" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D41" s="0" t="n">
+      <c r="D41" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F41" s="0" t="s">
+      <c r="E41" s="2"/>
+      <c r="F41" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C42" s="0" t="s">
+      <c r="B42" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D42" s="0" t="n">
+      <c r="D42" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="F42" s="0" t="s">
+      <c r="E42" s="2"/>
+      <c r="F42" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B43" s="0" t="n">
+      <c r="B43" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D43" s="0" t="n">
+      <c r="D43" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="F43" s="0" t="s">
+      <c r="E43" s="2"/>
+      <c r="F43" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B44" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C44" s="0" t="s">
+      <c r="B44" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D44" s="0" t="n">
+      <c r="D44" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="F44" s="0" t="s">
+      <c r="E44" s="2"/>
+      <c r="F44" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="0" t="n">
+      <c r="B45" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="0" t="n">
+      <c r="D45" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F45" s="0" t="s">
+      <c r="E45" s="2"/>
+      <c r="F45" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="0" t="n">
+      <c r="B46" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D46" s="0" t="n">
+      <c r="D46" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="F46" s="0" t="s">
+      <c r="E46" s="2"/>
+      <c r="F46" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="0" t="n">
+      <c r="B47" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D47" s="0" t="n">
+      <c r="D47" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F47" s="0" t="s">
+      <c r="E47" s="2"/>
+      <c r="F47" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1348,7 +1359,8 @@
       <c r="D48" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F48" s="0" t="s">
+      <c r="E48" s="2"/>
+      <c r="F48" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1365,166 +1377,173 @@
       <c r="D49" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F49" s="0" t="s">
+      <c r="E49" s="2"/>
+      <c r="F49" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B50" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C50" s="2" t="s">
+      <c r="B50" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D50" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F50" s="0" t="s">
+      <c r="D50" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B51" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="B51" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D51" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F51" s="0" t="s">
+      <c r="D51" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B52" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="B52" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D52" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F52" s="0" t="s">
+      <c r="D52" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B53" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C53" s="0" t="s">
+      <c r="B53" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D53" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F53" s="0" t="s">
+      <c r="D53" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B54" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C54" s="0" t="s">
+      <c r="B54" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D54" s="0" t="n">
+      <c r="D54" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F54" s="0" t="s">
+      <c r="E54" s="2"/>
+      <c r="F54" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B55" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C55" s="0" t="s">
+      <c r="B55" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D55" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E55" s="0" t="s">
+      <c r="D55" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F55" s="0" t="s">
+      <c r="F55" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B56" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C56" s="0" t="s">
+      <c r="B56" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D56" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E56" s="0" t="s">
+      <c r="D56" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E56" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F56" s="0" t="s">
+      <c r="F56" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B57" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C57" s="0" t="s">
+      <c r="B57" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D57" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F57" s="0" t="s">
+      <c r="D57" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="8"/>
+      <c r="B61" s="5"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="8"/>
+      <c r="B62" s="5"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="8"/>
+      <c r="B63" s="5"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="9"/>
+      <c r="B64" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
+  <autoFilter ref="A1:F57"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>